<commit_message>
updated graphs with new simulations
</commit_message>
<xml_diff>
--- a/channel database.xlsx
+++ b/channel database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akubo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akubo/myprojects/channelized-pdcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="16280" windowWidth="41500" windowHeight="10900" tabRatio="993"/>
+    <workbookView xWindow="5040" yWindow="2140" windowWidth="41500" windowHeight="23440" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="channels" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="157">
   <si>
     <t>channel label</t>
   </si>
@@ -448,6 +448,66 @@
   <si>
     <t>starts U shaped</t>
   </si>
+  <si>
+    <t>amprat</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>width/depth</t>
+  </si>
+  <si>
+    <t>300/39</t>
+  </si>
+  <si>
+    <t>100/15</t>
+  </si>
+  <si>
+    <t>200/27</t>
+  </si>
+  <si>
+    <t>volume flux</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Wavelength (m)</t>
+  </si>
+  <si>
+    <t>Width/Depth (m)</t>
+  </si>
+  <si>
+    <t>Inlet Height/Depth</t>
+  </si>
 </sst>
 </file>
 
@@ -456,7 +516,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -542,6 +602,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -933,7 +999,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1010,6 +1076,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="18"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="18" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="19" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
@@ -1691,11 +1758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-153610512"/>
-        <c:axId val="-268433584"/>
+        <c:axId val="-320342720"/>
+        <c:axId val="-320339200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-153610512"/>
+        <c:axId val="-320342720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.09"/>
@@ -1748,7 +1815,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1783,12 +1849,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-268433584"/>
+        <c:crossAx val="-320339200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-268433584"/>
+        <c:axId val="-320339200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -1841,7 +1907,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1876,7 +1941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153610512"/>
+        <c:crossAx val="-320342720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1889,7 +1954,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1935,10 +1999,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127892002309161"/>
-          <c:y val="0.0374978694392364"/>
-          <c:w val="0.827923087170833"/>
-          <c:h val="0.782853246974604"/>
+          <c:x val="0.139975064998252"/>
+          <c:y val="0.0435111268939394"/>
+          <c:w val="0.803786243177084"/>
+          <c:h val="0.761806818181818"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2558,6 +2622,141 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>our topograpy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(charts!$Y$53:$Y$61,charts!$Y$53:$Y$61,charts!$Y$53:$Y$61)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(charts!$Z$53:$Z$61,charts!$AA$53:$AA$61,charts!$AB$53:$AB$61)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>216.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>240.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2566,14 +2765,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121625360"/>
-        <c:axId val="-121621600"/>
+        <c:axId val="-390953920"/>
+        <c:axId val="-390950800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121625360"/>
+        <c:axId val="-390953920"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:min val="5.0"/>
+          <c:min val="100.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2584,7 +2784,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2598,7 +2798,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2635,7 +2835,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2651,15 +2851,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121621600"/>
+        <c:crossAx val="-390950800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-121621600"/>
+        <c:axId val="-390950800"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0"/>
+          <c:min val="10.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2670,7 +2871,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2684,7 +2885,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2705,8 +2906,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0383676006927483"/>
-              <c:y val="0.236236577467189"/>
+              <c:x val="0.0262992048167125"/>
+              <c:y val="0.260289535984848"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2728,7 +2929,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2744,7 +2945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121625360"/>
+        <c:crossAx val="-390953920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3287,11 +3488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121583792"/>
-        <c:axId val="-121580032"/>
+        <c:axId val="-390914112"/>
+        <c:axId val="-390910992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121583792"/>
+        <c:axId val="-390914112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -3379,12 +3580,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121580032"/>
+        <c:crossAx val="-390910992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-121580032"/>
+        <c:axId val="-390910992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -3472,7 +3673,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121583792"/>
+        <c:crossAx val="-390914112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3514,7 +3715,15 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="18"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -3523,10 +3732,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127930238522698"/>
-          <c:y val="0.0375072129255626"/>
-          <c:w val="0.820107719928187"/>
-          <c:h val="0.728793998845932"/>
+          <c:x val="0.139975064998252"/>
+          <c:y val="0.0435111268939394"/>
+          <c:w val="0.803786243177084"/>
+          <c:h val="0.761806818181818"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3539,16 +3748,16 @@
             <c:v>'Our Topography'</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750">
+            <a:ln w="25560">
               <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
+                <a:srgbClr val="283A7F"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -3996,14 +4205,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121539520"/>
-        <c:axId val="-121535760"/>
+        <c:axId val="-762743072"/>
+        <c:axId val="-762739040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121539520"/>
+        <c:axId val="-762743072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.35"/>
+          <c:max val="1.5"/>
           <c:min val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4015,7 +4224,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -4029,20 +4238,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Sinuosity</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Slope</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4066,7 +4269,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -4082,15 +4285,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121535760"/>
+        <c:crossAx val="-762739040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-121535760"/>
+        <c:axId val="-762739040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4101,7 +4303,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -4115,19 +4317,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Aspect Ratio</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Aspect Ratio</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4136,8 +4327,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0366760707873814"/>
-              <c:y val="0.319869205616465"/>
+              <c:x val="0.0234948617962295"/>
+              <c:y val="0.209395738269019"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4159,7 +4350,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -4175,7 +4366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121539520"/>
+        <c:crossAx val="-762743072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4189,26 +4380,6 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.212791879700973"/>
-          <c:y val="0.887386035884036"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
@@ -4738,11 +4909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121496512"/>
-        <c:axId val="-121492752"/>
+        <c:axId val="-390773696"/>
+        <c:axId val="-390770576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121496512"/>
+        <c:axId val="-390773696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000.0"/>
@@ -4824,12 +4995,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121492752"/>
+        <c:crossAx val="-390770576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-121492752"/>
+        <c:axId val="-390770576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -4917,7 +5088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121496512"/>
+        <c:crossAx val="-390773696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5487,13 +5658,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121450000"/>
-        <c:axId val="-121446240"/>
+        <c:axId val="-390803360"/>
+        <c:axId val="-390800240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121450000"/>
+        <c:axId val="-390803360"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
+          <c:min val="100.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5571,13 +5744,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121446240"/>
+        <c:crossAx val="-390800240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-121446240"/>
+        <c:axId val="-390800240"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:max val="2600.0"/>
           <c:min val="500.0"/>
@@ -5665,7 +5839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121450000"/>
+        <c:crossAx val="-390803360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5727,7 +5901,15 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="18"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -5736,10 +5918,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127891543420554"/>
-          <c:y val="0.0375"/>
-          <c:w val="0.830204778156996"/>
-          <c:h val="0.825968309859155"/>
+          <c:x val="0.139975064998252"/>
+          <c:y val="0.0435111268939394"/>
+          <c:w val="0.803786243177084"/>
+          <c:h val="0.761806818181818"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6259,14 +6441,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121407328"/>
-        <c:axId val="-121403568"/>
+        <c:axId val="-804879360"/>
+        <c:axId val="-800061888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121407328"/>
+        <c:axId val="-804879360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="5.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -6277,7 +6458,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -6291,7 +6472,67 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US"/>
+                  <a:t>Title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12600">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-800061888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-800061888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -6302,8 +6543,11 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                     <a:ea typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Average Slope</a:t>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Title</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6312,8 +6556,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.499478574137277"/>
-              <c:y val="0.933978873239437"/>
+              <c:x val="0.0262992048167125"/>
+              <c:y val="0.260289535984848"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -6335,7 +6579,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -6351,100 +6595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121403568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-121403568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="10.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Ratio of Wavelengths</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.0207622298065984"/>
-              <c:y val="0.347447183098592"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="12600">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-121407328"/>
+        <c:crossAx val="-804879360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6712,11 +6863,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-120578704"/>
-        <c:axId val="-120576224"/>
+        <c:axId val="-826068672"/>
+        <c:axId val="-826066624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-120578704"/>
+        <c:axId val="-826068672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6753,12 +6904,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120576224"/>
+        <c:crossAx val="-826066624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-120576224"/>
+        <c:axId val="-826066624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6804,7 +6955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120578704"/>
+        <c:crossAx val="-826068672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7079,11 +7230,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-120550416"/>
-        <c:axId val="-120547936"/>
+        <c:axId val="-826040304"/>
+        <c:axId val="-826037824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-120550416"/>
+        <c:axId val="-826040304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7120,12 +7271,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120547936"/>
+        <c:crossAx val="-826037824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-120547936"/>
+        <c:axId val="-826037824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7171,7 +7322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120550416"/>
+        <c:crossAx val="-826040304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8431,13 +8582,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.555555555555555</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.571428571428571</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.142857142857143</c:v>
+                  <c:v>1200.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8449,13 +8594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>18.0</c:v>
+                  <c:v>900.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8470,11 +8615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-120518320"/>
-        <c:axId val="-120514560"/>
+        <c:axId val="-826008464"/>
+        <c:axId val="-826004704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-120518320"/>
+        <c:axId val="-826008464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8578,12 +8723,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120514560"/>
+        <c:crossAx val="-826004704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-120514560"/>
+        <c:axId val="-826004704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8703,7 +8848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120518320"/>
+        <c:crossAx val="-826008464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10013,13 +10158,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.555555555555555</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.571428571428571</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.142857142857143</c:v>
+                  <c:v>1200.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10031,13 +10170,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>600.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500.0</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10052,11 +10191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-120486384"/>
-        <c:axId val="-120482624"/>
+        <c:axId val="-825976528"/>
+        <c:axId val="-825972768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-120486384"/>
+        <c:axId val="-825976528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -10165,12 +10304,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120482624"/>
+        <c:crossAx val="-825972768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-120482624"/>
+        <c:axId val="-825972768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -10291,7 +10430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120486384"/>
+        <c:crossAx val="-825976528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10906,11 +11045,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-310442160"/>
-        <c:axId val="-310437968"/>
+        <c:axId val="-453444512"/>
+        <c:axId val="-453371376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-310442160"/>
+        <c:axId val="-453444512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.09"/>
@@ -10998,12 +11137,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-310437968"/>
+        <c:crossAx val="-453371376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-310437968"/>
+        <c:axId val="-453371376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -11091,7 +11230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-310442160"/>
+        <c:crossAx val="-453444512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11285,11 +11424,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-153605888"/>
-        <c:axId val="-153602768"/>
+        <c:axId val="-320259008"/>
+        <c:axId val="-320255888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-153605888"/>
+        <c:axId val="-320259008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11369,7 +11508,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153602768"/>
+        <c:crossAx val="-320255888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11377,7 +11516,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-153602768"/>
+        <c:axId val="-320255888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11457,7 +11596,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153605888"/>
+        <c:crossAx val="-320259008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -11652,11 +11791,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-153575696"/>
-        <c:axId val="-153572576"/>
+        <c:axId val="-320230384"/>
+        <c:axId val="-320227264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-153575696"/>
+        <c:axId val="-320230384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11736,7 +11875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153572576"/>
+        <c:crossAx val="-320227264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11744,7 +11883,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-153572576"/>
+        <c:axId val="-320227264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11824,7 +11963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153575696"/>
+        <c:crossAx val="-320230384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -11989,11 +12128,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-153999040"/>
-        <c:axId val="-153995920"/>
+        <c:axId val="-320205344"/>
+        <c:axId val="-320202224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-153999040"/>
+        <c:axId val="-320205344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12073,7 +12212,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153995920"/>
+        <c:crossAx val="-320202224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12081,7 +12220,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-153995920"/>
+        <c:axId val="-320202224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12158,7 +12297,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153999040"/>
+        <c:crossAx val="-320205344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -12368,11 +12507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-313560096"/>
-        <c:axId val="-313558304"/>
+        <c:axId val="-320167248"/>
+        <c:axId val="-320165200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-313560096"/>
+        <c:axId val="-320167248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12429,12 +12568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-313558304"/>
+        <c:crossAx val="-320165200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-313558304"/>
+        <c:axId val="-320165200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12490,7 +12629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-313560096"/>
+        <c:crossAx val="-320167248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12660,11 +12799,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-311474544"/>
-        <c:axId val="-311471152"/>
+        <c:axId val="-314318208"/>
+        <c:axId val="-314314816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-311474544"/>
+        <c:axId val="-314318208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12757,7 +12896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-311471152"/>
+        <c:crossAx val="-314314816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12765,7 +12904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-311471152"/>
+        <c:axId val="-314314816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12860,7 +12999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-311474544"/>
+        <c:crossAx val="-314318208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15.0"/>
@@ -14351,6 +14490,103 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Our Topography</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="10"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="10"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="diamond"/>
+              <c:size val="10"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+                <a:ln w="12700">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>charts!$C$48:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>charts!$D$48:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -14359,12 +14595,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-153503968"/>
-        <c:axId val="-153500208"/>
+        <c:axId val="-826153264"/>
+        <c:axId val="-826150144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-153503968"/>
+        <c:axId val="-826153264"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
         </c:scaling>
@@ -14377,7 +14614,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -14391,7 +14628,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -14435,7 +14672,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -14451,13 +14688,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153500208"/>
+        <c:crossAx val="-826150144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-153500208"/>
+        <c:axId val="-826150144"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
         </c:scaling>
@@ -14470,7 +14708,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -14484,7 +14722,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -14505,8 +14743,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0314241032157169"/>
-              <c:y val="0.353795730356985"/>
+              <c:x val="0.01542328464517"/>
+              <c:y val="0.2944153517536"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -14528,7 +14766,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -14544,7 +14782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153503968"/>
+        <c:crossAx val="-826153264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14564,8 +14802,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.667571505484891"/>
-          <c:y val="0.426170767716535"/>
+          <c:x val="0.706801518202194"/>
+          <c:y val="0.416795040899292"/>
+          <c:w val="0.199275607574434"/>
+          <c:h val="0.357467196897363"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -14577,6 +14817,20 @@
           </a:solidFill>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Arial" charset="0"/>
+              <a:ea typeface="Arial" charset="0"/>
+              <a:cs typeface="Arial" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -14606,7 +14860,15 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="18"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -14615,10 +14877,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127897915449055"/>
-          <c:y val="0.0375"/>
-          <c:w val="0.830216247808299"/>
-          <c:h val="0.825968309859155"/>
+          <c:x val="0.139975064998252"/>
+          <c:y val="0.0435111268939394"/>
+          <c:w val="0.803786243177084"/>
+          <c:h val="0.761806818181818"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -14734,83 +14996,6 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Our topography</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25560">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>sims!$A$3:$A$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>17.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>sims!$B$3:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>400.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>600.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>800.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
             <c:strRef>
               <c:f>channels!$A$9</c:f>
               <c:strCache>
@@ -14902,8 +15087,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>channels!$A$14</c:f>
@@ -14996,8 +15181,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>channels!$A$19</c:f>
@@ -15102,8 +15287,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>channels!$A$26</c:f>
@@ -15201,6 +15386,81 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Our Topography</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(charts!$X$55,charts!$X$57,charts!$X$59:$X$61)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(charts!$Y$55,charts!$Y$57,charts!$Y$59:$Y$61)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -15209,12 +15469,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-153459392"/>
-        <c:axId val="-153455632"/>
+        <c:axId val="-797748816"/>
+        <c:axId val="-825424096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-153459392"/>
+        <c:axId val="-797748816"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
         </c:scaling>
@@ -15227,7 +15488,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -15241,7 +15502,69 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Slope</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12600">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-825424096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-825424096"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -15252,8 +15575,11 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                     <a:ea typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Average Slope</a:t>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Wavelength</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -15262,8 +15588,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.499464250925385"/>
-              <c:y val="0.933978873239437"/>
+              <c:x val="0.016355455568054"/>
+              <c:y val="0.313087156412012"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -15285,7 +15611,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="1100" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -15301,100 +15627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-153455632"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-153455632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="1.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Arial"/>
-                    <a:ea typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Wavelength (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.0207481005260082"/>
-              <c:y val="0.347535211267606"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="12600">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-                <a:ea typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-153459392"/>
+        <c:crossAx val="-797748816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17873,16 +18106,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>622440</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>444640</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>787320</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>177400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17903,16 +18136,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>177840</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152460</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>367920</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>177660</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17933,16 +18166,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>594000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>174900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>5280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>470880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>51780</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>165280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18083,16 +18316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>774720</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>88920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>139320</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>139680</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>228220</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18173,15 +18406,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>127360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>445400</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>420000</xdr:colOff>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -18749,6 +18982,762 @@
 
 <file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
 <a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride4.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride5.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <a:clrScheme name="Slipstream">
     <a:dk1>
       <a:sysClr val="windowText" lastClr="000000"/>
@@ -18999,7 +19988,7 @@
 </a:themeOverride>
 </file>
 
-<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/themeOverride6.xml><?xml version="1.0" encoding="utf-8"?>
 <a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <a:clrScheme name="Slipstream">
     <a:dk1>
@@ -19255,9 +20244,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27588,7 +28577,7 @@
         <v>4710</v>
       </c>
       <c r="F33" s="75">
-        <f t="shared" ref="F32:F37" si="14">E33/D33</f>
+        <f t="shared" ref="F33:F37" si="14">E33/D33</f>
         <v>1.0726485994078798</v>
       </c>
       <c r="G33" s="56">
@@ -43559,10 +44548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43571,7 +44560,7 @@
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>48</v>
       </c>
@@ -43614,8 +44603,11 @@
       <c r="P1" t="s">
         <v>99</v>
       </c>
+      <c r="Q1" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -43667,7 +44659,7 @@
         <v>1144.4305555555541</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -43719,7 +44711,7 @@
         <v>872.75</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -43771,7 +44763,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -43823,7 +44815,7 @@
         <v>1106.5833333333335</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -43875,7 +44867,7 @@
         <v>547.70000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -43926,8 +44918,12 @@
         <f>AVERAGE(channels!P2:P30,channels!S2:S30)</f>
         <v>995.9108527131782</v>
       </c>
+      <c r="Q7">
+        <f>AVERAGE(channels!AA3:AB8,channels!AA10:AB13,channels!AB20:AB25,channels!AA22,channels!AA24:AA25,channels!AA27:AB31,channels!AA15,channels!AA17,channels!AB15:AB18)</f>
+        <v>0.16296142376370804</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -43977,6 +44973,10 @@
       <c r="P8">
         <f>_xlfn.STDEV.P(channels!P3:P31,channels!S3:S31)</f>
         <v>849.44941273809673</v>
+      </c>
+      <c r="Q8">
+        <f>_xlfn.STDEV.P(channels!AA4:AB9,channels!AA11:AB14,channels!AB21:AB26,channels!AA23,channels!AA25:AA26,channels!AA28:AB32,channels!AA16,channels!AA18,channels!AB16:AB19)</f>
+        <v>6.2163350124394799E-2</v>
       </c>
     </row>
   </sheetData>
@@ -49691,10 +50691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49702,82 +50702,210 @@
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="76"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
-      </c>
+      <c r="B3" s="76">
+        <v>300</v>
+      </c>
+      <c r="C3" s="76">
+        <v>600</v>
+      </c>
+      <c r="D3" s="76">
+        <v>900</v>
+      </c>
+      <c r="E3" s="76">
+        <v>1200</v>
+      </c>
+      <c r="F3" s="76">
+        <v>2400</v>
+      </c>
+      <c r="G3" s="76">
+        <v>0</v>
+      </c>
+      <c r="H3" s="76"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <f>C3/D3</f>
-        <v>5.5555555555555554</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>400</v>
-      </c>
-      <c r="C4">
-        <v>300</v>
-      </c>
-      <c r="D4">
-        <v>35</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E5" si="0">C4/D4</f>
-        <v>8.5714285714285712</v>
-      </c>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="76">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="76">
+        <v>0.09</v>
+      </c>
+      <c r="D5" s="76">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>600</v>
-      </c>
-      <c r="C5">
-        <v>500</v>
-      </c>
-      <c r="D5">
-        <v>70</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>7.1428571428571432</v>
-      </c>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>800</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>1600</v>
-      </c>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="76">
+        <v>1</v>
+      </c>
+      <c r="C8" s="76">
+        <v>4</v>
+      </c>
+      <c r="D8" s="76">
+        <v>7</v>
+      </c>
+      <c r="E8" s="76">
+        <v>0</v>
+      </c>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -49790,7 +50918,7 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50478,17 +51606,160 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L49"/>
+  <dimension ref="C48:AB61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N87" sqref="N87"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="49" spans="12:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>100</v>
+      </c>
+      <c r="D48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>200</v>
+      </c>
+      <c r="D49">
+        <v>27</v>
+      </c>
       <c r="L49" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>300</v>
+      </c>
+      <c r="D50">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="Z52">
+        <v>0.09</v>
+      </c>
+      <c r="AA52">
+        <v>0.15</v>
+      </c>
+      <c r="AB52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X55">
+        <v>18</v>
+      </c>
+      <c r="Y55">
+        <v>300</v>
+      </c>
+      <c r="Z55">
+        <f t="shared" ref="Z54:AB61" si="0">$Y55*Z$52</f>
+        <v>27</v>
+      </c>
+      <c r="AA55">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AB55">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X56">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X57">
+        <v>18</v>
+      </c>
+      <c r="Y57">
+        <v>600</v>
+      </c>
+      <c r="Z57">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="AA57">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="AB57">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X59">
+        <v>18</v>
+      </c>
+      <c r="Y59">
+        <v>2400</v>
+      </c>
+      <c r="Z59">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="AA59">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="AB59">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="60" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X60">
+        <v>18</v>
+      </c>
+      <c r="Y60">
+        <v>900</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="3:28" x14ac:dyDescent="0.2">
+      <c r="X61">
+        <v>18</v>
+      </c>
+      <c r="Y61">
+        <v>1200</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="0"/>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated histograms in channel database
</commit_message>
<xml_diff>
--- a/channel database.xlsx
+++ b/channel database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="2140" windowWidth="41500" windowHeight="23440" tabRatio="993" activeTab="6"/>
+    <workbookView xWindow="24200" yWindow="2140" windowWidth="22340" windowHeight="23440" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="channels" sheetId="1" r:id="rId1"/>
@@ -977,7 +977,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -998,6 +998,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1078,7 +1082,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="19" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="24">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
     <cellStyle name="40% - Accent1" xfId="19" builtinId="31"/>
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1089,6 +1093,8 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1096,6 +1102,8 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1758,11 +1766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-320342720"/>
-        <c:axId val="-320339200"/>
+        <c:axId val="-763118112"/>
+        <c:axId val="-763303296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-320342720"/>
+        <c:axId val="-763118112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.09"/>
@@ -1849,12 +1857,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320339200"/>
+        <c:crossAx val="-763303296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-320339200"/>
+        <c:axId val="-763303296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -1941,7 +1949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320342720"/>
+        <c:crossAx val="-763118112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2765,11 +2773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-390953920"/>
-        <c:axId val="-390950800"/>
+        <c:axId val="-762851376"/>
+        <c:axId val="-762848256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-390953920"/>
+        <c:axId val="-762851376"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2851,12 +2859,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390950800"/>
+        <c:crossAx val="-762848256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-390950800"/>
+        <c:axId val="-762848256"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2945,7 +2953,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390953920"/>
+        <c:crossAx val="-762851376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3488,11 +3496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-390914112"/>
-        <c:axId val="-390910992"/>
+        <c:axId val="-323206928"/>
+        <c:axId val="-763185056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-390914112"/>
+        <c:axId val="-323206928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -3580,12 +3588,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390910992"/>
+        <c:crossAx val="-763185056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-390910992"/>
+        <c:axId val="-763185056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -3673,7 +3681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390914112"/>
+        <c:crossAx val="-323206928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4205,11 +4213,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-762743072"/>
-        <c:axId val="-762739040"/>
+        <c:axId val="-797752080"/>
+        <c:axId val="-797748960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-762743072"/>
+        <c:axId val="-797752080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -4285,12 +4293,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-762739040"/>
+        <c:crossAx val="-797748960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-762739040"/>
+        <c:axId val="-797748960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4366,7 +4374,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-762743072"/>
+        <c:crossAx val="-797752080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4909,11 +4917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-390773696"/>
-        <c:axId val="-390770576"/>
+        <c:axId val="-797764176"/>
+        <c:axId val="-519089088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-390773696"/>
+        <c:axId val="-797764176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000.0"/>
@@ -4995,12 +5003,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390770576"/>
+        <c:crossAx val="-519089088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-390770576"/>
+        <c:axId val="-519089088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -5088,7 +5096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390773696"/>
+        <c:crossAx val="-797764176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5658,11 +5666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-390803360"/>
-        <c:axId val="-390800240"/>
+        <c:axId val="-797715952"/>
+        <c:axId val="-797759952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-390803360"/>
+        <c:axId val="-797715952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5744,12 +5752,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390800240"/>
+        <c:crossAx val="-797759952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-390800240"/>
+        <c:axId val="-797759952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5839,7 +5847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-390803360"/>
+        <c:crossAx val="-797715952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6441,11 +6449,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-804879360"/>
-        <c:axId val="-800061888"/>
+        <c:axId val="-763078160"/>
+        <c:axId val="-763258032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-804879360"/>
+        <c:axId val="-763078160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6514,12 +6522,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-800061888"/>
+        <c:crossAx val="-763258032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-800061888"/>
+        <c:axId val="-763258032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6595,7 +6603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804879360"/>
+        <c:crossAx val="-763078160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6863,11 +6871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-826068672"/>
-        <c:axId val="-826066624"/>
+        <c:axId val="-762879920"/>
+        <c:axId val="-762877872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-826068672"/>
+        <c:axId val="-762879920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6904,12 +6912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826066624"/>
+        <c:crossAx val="-762877872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-826066624"/>
+        <c:axId val="-762877872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6955,7 +6963,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826068672"/>
+        <c:crossAx val="-762879920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7230,11 +7238,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-826040304"/>
-        <c:axId val="-826037824"/>
+        <c:axId val="-322990528"/>
+        <c:axId val="-763344208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-826040304"/>
+        <c:axId val="-322990528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7271,12 +7279,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826037824"/>
+        <c:crossAx val="-763344208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-826037824"/>
+        <c:axId val="-763344208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7322,7 +7330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826040304"/>
+        <c:crossAx val="-322990528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8615,11 +8623,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-826008464"/>
-        <c:axId val="-826004704"/>
+        <c:axId val="-763272608"/>
+        <c:axId val="-763268928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-826008464"/>
+        <c:axId val="-763272608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8660,7 +8668,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8723,12 +8730,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826004704"/>
+        <c:crossAx val="-763268928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-826004704"/>
+        <c:axId val="-763268928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8848,7 +8855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826008464"/>
+        <c:crossAx val="-763272608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10191,11 +10198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-825976528"/>
-        <c:axId val="-825972768"/>
+        <c:axId val="-763018448"/>
+        <c:axId val="-763016016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-825976528"/>
+        <c:axId val="-763018448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -10304,12 +10311,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-825972768"/>
+        <c:crossAx val="-763016016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-825972768"/>
+        <c:axId val="-763016016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -10430,7 +10437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-825976528"/>
+        <c:crossAx val="-763018448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11045,11 +11052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-453444512"/>
-        <c:axId val="-453371376"/>
+        <c:axId val="-763170256"/>
+        <c:axId val="-763136192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-453444512"/>
+        <c:axId val="-763170256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.09"/>
@@ -11102,7 +11109,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -11137,12 +11143,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-453371376"/>
+        <c:crossAx val="-763136192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-453371376"/>
+        <c:axId val="-763136192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -11195,7 +11201,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -11230,7 +11235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-453444512"/>
+        <c:crossAx val="-763170256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11243,7 +11248,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11378,28 +11382,28 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.0</c:v>
@@ -11408,7 +11412,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11424,11 +11428,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-320259008"/>
-        <c:axId val="-320255888"/>
+        <c:axId val="-325016192"/>
+        <c:axId val="-799757104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-320259008"/>
+        <c:axId val="-325016192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11508,7 +11512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320255888"/>
+        <c:crossAx val="-799757104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11516,7 +11520,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-320255888"/>
+        <c:axId val="-799757104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11596,7 +11600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320259008"/>
+        <c:crossAx val="-325016192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -11691,43 +11695,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>13.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.0</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.0</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.0</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63.0</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83.0</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93.0</c:v>
+                  <c:v>135.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>103.0</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>113.0</c:v>
+                  <c:v>165.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>123.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>133.0</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11739,43 +11740,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>50.0</c:v>
+                  <c:v>58.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.0</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11791,11 +11789,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-320230384"/>
-        <c:axId val="-320227264"/>
+        <c:axId val="-325052432"/>
+        <c:axId val="-325048976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-320230384"/>
+        <c:axId val="-325052432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11875,7 +11873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320227264"/>
+        <c:crossAx val="-325048976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11883,7 +11881,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-320227264"/>
+        <c:axId val="-325048976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11963,7 +11961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320230384"/>
+        <c:crossAx val="-325052432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -12058,28 +12056,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.05931952662722</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.11863905325444</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.17795857988165</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60.23727810650887</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75.29659763313608</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.35591715976331</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105.4152366863905</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12091,28 +12089,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>29.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>12.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12128,11 +12126,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-320205344"/>
-        <c:axId val="-320202224"/>
+        <c:axId val="-799833248"/>
+        <c:axId val="-799830128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-320205344"/>
+        <c:axId val="-799833248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12212,7 +12210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320202224"/>
+        <c:crossAx val="-799830128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12220,7 +12218,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-320202224"/>
+        <c:axId val="-799830128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12297,7 +12295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320205344"/>
+        <c:crossAx val="-799833248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -12507,11 +12505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-320167248"/>
-        <c:axId val="-320165200"/>
+        <c:axId val="-554757536"/>
+        <c:axId val="-554756176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-320167248"/>
+        <c:axId val="-554757536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12568,12 +12566,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320165200"/>
+        <c:crossAx val="-554756176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-320165200"/>
+        <c:axId val="-554756176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12629,7 +12627,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-320167248"/>
+        <c:crossAx val="-554757536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12799,11 +12797,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-314318208"/>
-        <c:axId val="-314314816"/>
+        <c:axId val="-519166816"/>
+        <c:axId val="-797883872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-314318208"/>
+        <c:axId val="-519166816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12896,7 +12894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-314314816"/>
+        <c:crossAx val="-797883872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12904,7 +12902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-314314816"/>
+        <c:axId val="-797883872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12999,7 +12997,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-314318208"/>
+        <c:crossAx val="-519166816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15.0"/>
@@ -14595,11 +14593,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-826153264"/>
-        <c:axId val="-826150144"/>
+        <c:axId val="-800315552"/>
+        <c:axId val="-800180480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-826153264"/>
+        <c:axId val="-800315552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -14688,12 +14686,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826150144"/>
+        <c:crossAx val="-800180480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-826150144"/>
+        <c:axId val="-800180480"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -14782,7 +14780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-826153264"/>
+        <c:crossAx val="-800315552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15469,11 +15467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-797748816"/>
-        <c:axId val="-825424096"/>
+        <c:axId val="-323625728"/>
+        <c:axId val="-763249712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-797748816"/>
+        <c:axId val="-323625728"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -15544,12 +15542,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-825424096"/>
+        <c:crossAx val="-763249712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-825424096"/>
+        <c:axId val="-763249712"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -15627,7 +15625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797748816"/>
+        <c:crossAx val="-323625728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17946,16 +17944,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>89040</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>190520</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>343040</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>177820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>342840</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>50680</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>596840</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>37980</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17976,16 +17974,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>177820</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>6240</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>20</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>469680</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>82200</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>291880</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>56800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18006,16 +18004,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>38160</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>622360</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>69520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>482400</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:colOff>393500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>145840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20245,8 +20243,8 @@
   <dimension ref="A1:AMK55"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA3" sqref="AA3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34816,7 +34814,10 @@
       <c r="A39" s="46"/>
       <c r="B39" s="46"/>
       <c r="C39" s="55"/>
-      <c r="D39" s="46"/>
+      <c r="D39" s="46">
+        <f>COUNT(D3:D37)</f>
+        <v>30</v>
+      </c>
       <c r="E39" s="46"/>
       <c r="F39" s="46"/>
       <c r="G39" s="57"/>
@@ -44989,8 +44990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="V52" sqref="V52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47494,10 +47495,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y217"/>
+  <dimension ref="A1:Y234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47520,19 +47521,19 @@
         <v>89</v>
       </c>
       <c r="F1">
-        <f>(G22-H22)/(L1)</f>
-        <v>102.14285714285714</v>
+        <f>(H49-I49)/(L1)</f>
+        <v>89.375</v>
       </c>
       <c r="H1">
-        <f>(G21-H21)/(L1)</f>
-        <v>12.071428571428571</v>
+        <f>(H48-I48)/(L1)</f>
+        <v>10.5625</v>
       </c>
       <c r="K1">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="L1">
         <f>_xlfn.CEILING.MATH(SQRT(K1))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O1" t="s">
         <v>114</v>
@@ -47607,31 +47608,34 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="array" ref="F3:F16">FREQUENCY(B1:B184,E3:E13)</f>
+        <f t="array" ref="F3:F15">FREQUENCY(B1:B234,E3:E15)</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f>100*F3/$K$1</f>
+        <f>F3/$K$1*100</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>0</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="array" ref="I3:I16">FREQUENCY(C1:C197,H3:H16)</f>
+        <f t="array" ref="I3:I15">FREQUENCY(C1:C234,H3:H15)</f>
         <v>0</v>
       </c>
+      <c r="J3">
+        <f>I3/$K$1*100</f>
+        <v>0</v>
+      </c>
       <c r="K3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <f t="array" ref="L3:L16">FREQUENCY(D1:D184,K3:K16)</f>
-        <v>29</v>
+        <f t="array" ref="L3:L15">FREQUENCY(D1:D234,K3:K15)</f>
+        <v>0</v>
       </c>
       <c r="M3">
-        <f>100*L3/K$1</f>
-        <v>15.760869565217391</v>
+        <f>L3/$K$1*100</f>
+        <v>0</v>
       </c>
       <c r="O3" s="35">
         <f t="shared" ref="O3:O16" si="1">G3*O$2/100</f>
@@ -47643,7 +47647,7 @@
       </c>
       <c r="Q3" s="36">
         <f t="shared" ref="Q3:Q16" si="3">M3*O$2/100</f>
-        <v>0.47282608695652173</v>
+        <v>0</v>
       </c>
       <c r="T3" s="38" t="s">
         <v>123</v>
@@ -47664,45 +47668,43 @@
         <v>100</v>
       </c>
       <c r="F4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G14" si="4">100*F4/$K$1</f>
-        <v>6.5217391304347823</v>
+        <f t="shared" ref="G4:G15" si="4">F4/$K$1*100</f>
+        <v>7.296137339055794</v>
       </c>
       <c r="H4">
-        <f>_xlfn.CEILING.MATH(H1+H3)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J4">
-        <f>100*I4/$K$1</f>
-        <v>27.173913043478262</v>
+        <f t="shared" ref="J4:J15" si="5">I4/$K$1*100</f>
+        <v>24.892703862660944</v>
       </c>
       <c r="K4">
-        <f>(MAX(D1:D184)-MIN(D1:D184))/H1</f>
-        <v>15.059319526627219</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M16" si="5">100*L4/K$1</f>
-        <v>53.260869565217391</v>
+        <f t="shared" ref="M4:M15" si="6">L4/$K$1*100</f>
+        <v>0</v>
       </c>
       <c r="O4" s="37">
         <f t="shared" si="1"/>
-        <v>0.19565217391304349</v>
+        <v>0.21888412017167383</v>
       </c>
       <c r="P4" s="36">
         <f t="shared" si="2"/>
-        <v>0.81521739130434778</v>
+        <v>0.74678111587982843</v>
       </c>
       <c r="Q4" s="36">
         <f t="shared" si="3"/>
-        <v>1.597826086956522</v>
+        <v>0</v>
       </c>
       <c r="S4" s="40" t="s">
         <v>120</v>
@@ -47736,49 +47738,48 @@
         <v>17.285714285714285</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E16" si="6">E4+100</f>
+        <f t="shared" ref="E5:E16" si="7">E4+100</f>
         <v>200</v>
       </c>
       <c r="F5">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>27.173913043478262</v>
+        <v>24.463519313304722</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H16" si="7">H4+10</f>
-        <v>23</v>
+        <f>H4+15</f>
+        <v>30</v>
       </c>
       <c r="I5">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J16" si="8">100*I5/$K$1</f>
-        <v>21.195652173913043</v>
+        <f t="shared" si="5"/>
+        <v>26.180257510729614</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K16" si="9">K4+$K$4</f>
-        <v>30.118639053254437</v>
+        <v>4</v>
       </c>
       <c r="L5">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="M5">
-        <f t="shared" si="5"/>
-        <v>17.391304347826086</v>
+        <f t="shared" si="6"/>
+        <v>4.7210300429184553</v>
       </c>
       <c r="O5" s="36">
         <f t="shared" si="1"/>
-        <v>0.81521739130434778</v>
+        <v>0.73390557939914169</v>
       </c>
       <c r="P5" s="36">
         <f t="shared" si="2"/>
-        <v>0.63586956521739124</v>
+        <v>0.78540772532188841</v>
       </c>
       <c r="Q5" s="36">
         <f t="shared" si="3"/>
-        <v>0.52173913043478259</v>
+        <v>0.14163090128755365</v>
       </c>
       <c r="R5" s="38" t="s">
         <v>117</v>
@@ -47815,49 +47816,48 @@
         <v>21.2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="F6">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G6">
         <f t="shared" si="4"/>
-        <v>28.804347826086957</v>
+        <v>26.609442060085836</v>
       </c>
       <c r="H6">
-        <f t="shared" si="7"/>
-        <v>33</v>
+        <f t="shared" ref="H6:H15" si="8">H5+15</f>
+        <v>45</v>
       </c>
       <c r="I6">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J6">
-        <f t="shared" si="8"/>
-        <v>15.217391304347826</v>
+        <f t="shared" si="5"/>
+        <v>12.875536480686694</v>
       </c>
       <c r="K6">
-        <f t="shared" si="9"/>
-        <v>45.177958579881654</v>
+        <v>6</v>
       </c>
       <c r="L6">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
-        <v>6.5217391304347823</v>
+        <f t="shared" si="6"/>
+        <v>17.167381974248926</v>
       </c>
       <c r="O6" s="36">
         <f t="shared" si="1"/>
-        <v>0.86413043478260876</v>
+        <v>0.79828326180257503</v>
       </c>
       <c r="P6" s="36">
         <f t="shared" si="2"/>
-        <v>0.45652173913043476</v>
+        <v>0.38626609442060089</v>
       </c>
       <c r="Q6" s="37">
         <f t="shared" si="3"/>
-        <v>0.19565217391304349</v>
+        <v>0.51502145922746778</v>
       </c>
       <c r="R6" s="40" t="s">
         <v>118</v>
@@ -47873,11 +47873,11 @@
         <v>30</v>
       </c>
       <c r="X6">
-        <f t="shared" ref="X6:Y6" si="10">X5/X4</f>
+        <f t="shared" ref="X6:Y6" si="9">X5/X4</f>
         <v>42.857142857142854</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
     </row>
@@ -47893,49 +47893,48 @@
         <v>38.1</v>
       </c>
       <c r="E7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>400</v>
       </c>
       <c r="F7">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G7">
         <f t="shared" si="4"/>
-        <v>19.565217391304348</v>
+        <v>17.167381974248926</v>
       </c>
       <c r="H7">
-        <f t="shared" si="7"/>
-        <v>43</v>
+        <f t="shared" si="8"/>
+        <v>60</v>
       </c>
       <c r="I7">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J7">
-        <f t="shared" si="8"/>
-        <v>11.413043478260869</v>
+        <f t="shared" si="5"/>
+        <v>8.1545064377682408</v>
       </c>
       <c r="K7">
-        <f t="shared" si="9"/>
-        <v>60.237278106508874</v>
+        <v>8</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="M7">
-        <f t="shared" si="5"/>
-        <v>2.1739130434782608</v>
+        <f t="shared" si="6"/>
+        <v>9.8712446351931327</v>
       </c>
       <c r="O7" s="36">
         <f t="shared" si="1"/>
-        <v>0.58695652173913049</v>
+        <v>0.51502145922746778</v>
       </c>
       <c r="P7" s="37">
         <f t="shared" si="2"/>
-        <v>0.34239130434782611</v>
+        <v>0.24463519313304721</v>
       </c>
       <c r="Q7" s="35">
         <f t="shared" si="3"/>
-        <v>6.5217391304347824E-2</v>
+        <v>0.29613733905579398</v>
       </c>
       <c r="R7" s="39" t="s">
         <v>119</v>
@@ -47953,49 +47952,48 @@
         <v>25.5</v>
       </c>
       <c r="E8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
       <c r="F8">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>6.5217391304347823</v>
+        <v>11.587982832618025</v>
       </c>
       <c r="H8">
-        <f t="shared" si="7"/>
-        <v>53</v>
+        <f t="shared" si="8"/>
+        <v>75</v>
       </c>
       <c r="I8">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J8">
-        <f t="shared" si="8"/>
-        <v>4.8913043478260869</v>
+        <f t="shared" si="5"/>
+        <v>7.296137339055794</v>
       </c>
       <c r="K8">
-        <f t="shared" si="9"/>
-        <v>75.296597633136088</v>
+        <v>10</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>10.300429184549357</v>
       </c>
       <c r="O8" s="37">
         <f t="shared" si="1"/>
-        <v>0.19565217391304349</v>
+        <v>0.34763948497854075</v>
       </c>
       <c r="P8" s="37">
         <f t="shared" si="2"/>
-        <v>0.14673913043478262</v>
+        <v>0.21888412017167383</v>
       </c>
       <c r="Q8" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.30901287553648066</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -48010,49 +48008,48 @@
         <v>5.0265486725663715</v>
       </c>
       <c r="E9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>600</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>5.4347826086956523</v>
+        <v>6.4377682403433472</v>
       </c>
       <c r="H9">
-        <f t="shared" si="7"/>
-        <v>63</v>
+        <f t="shared" si="8"/>
+        <v>90</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J9">
-        <f t="shared" si="8"/>
-        <v>5.4347826086956523</v>
+        <f t="shared" si="5"/>
+        <v>5.1502145922746783</v>
       </c>
       <c r="K9">
-        <f t="shared" si="9"/>
-        <v>90.355917159763308</v>
+        <v>12</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
-        <v>1.0869565217391304</v>
+        <f t="shared" si="6"/>
+        <v>5.1502145922746783</v>
       </c>
       <c r="O9" s="35">
         <f t="shared" si="1"/>
-        <v>0.16304347826086957</v>
+        <v>0.19313304721030045</v>
       </c>
       <c r="P9" s="35">
         <f t="shared" si="2"/>
-        <v>0.16304347826086957</v>
+        <v>0.15450643776824033</v>
       </c>
       <c r="Q9" s="35">
         <f t="shared" si="3"/>
-        <v>3.2608695652173912E-2</v>
+        <v>0.15450643776824033</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
@@ -48067,49 +48064,48 @@
         <v>7.0263157894736841</v>
       </c>
       <c r="E10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>700</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>2.1739130434782608</v>
+        <v>2.5751072961373391</v>
       </c>
       <c r="H10">
-        <f t="shared" si="7"/>
-        <v>73</v>
+        <f t="shared" si="8"/>
+        <v>105</v>
       </c>
       <c r="I10">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J10">
-        <f t="shared" si="8"/>
-        <v>3.8043478260869565</v>
+        <f t="shared" si="5"/>
+        <v>5.5793991416309012</v>
       </c>
       <c r="K10">
-        <f t="shared" si="9"/>
-        <v>105.41523668639053</v>
+        <v>14</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
-        <v>1.6304347826086956</v>
+        <f t="shared" si="6"/>
+        <v>4.7210300429184553</v>
       </c>
       <c r="O10" s="35">
         <f t="shared" si="1"/>
-        <v>6.5217391304347824E-2</v>
+        <v>7.7253218884120164E-2</v>
       </c>
       <c r="P10" s="35">
         <f t="shared" si="2"/>
-        <v>0.11413043478260869</v>
+        <v>0.16738197424892703</v>
       </c>
       <c r="Q10" s="35">
         <f t="shared" si="3"/>
-        <v>4.8913043478260872E-2</v>
+        <v>0.14163090128755365</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
@@ -48124,49 +48120,48 @@
         <v>25.357142857142858</v>
       </c>
       <c r="E11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>800</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>1.0869565217391304</v>
+        <v>2.1459227467811157</v>
       </c>
       <c r="H11">
-        <f t="shared" si="7"/>
-        <v>83</v>
+        <f t="shared" si="8"/>
+        <v>120</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J11">
-        <f t="shared" si="8"/>
-        <v>2.1739130434782608</v>
+        <f t="shared" si="5"/>
+        <v>3.4334763948497855</v>
       </c>
       <c r="K11">
-        <f t="shared" si="9"/>
-        <v>120.47455621301775</v>
+        <v>16</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
-        <v>0.54347826086956519</v>
+        <f t="shared" si="6"/>
+        <v>3.8626609442060089</v>
       </c>
       <c r="O11" s="35">
         <f t="shared" si="1"/>
-        <v>3.2608695652173912E-2</v>
+        <v>6.4377682403433473E-2</v>
       </c>
       <c r="P11" s="35">
         <f t="shared" si="2"/>
-        <v>6.5217391304347824E-2</v>
+        <v>0.10300429184549356</v>
       </c>
       <c r="Q11" s="35">
         <f t="shared" si="3"/>
-        <v>1.6304347826086956E-2</v>
+        <v>0.11587982832618027</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -48181,7 +48176,7 @@
         <v>7.6744186046511631</v>
       </c>
       <c r="E12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>900</v>
       </c>
       <c r="F12">
@@ -48189,41 +48184,40 @@
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>1.0869565217391304</v>
+        <v>0.85836909871244638</v>
       </c>
       <c r="H12">
-        <f t="shared" si="7"/>
-        <v>93</v>
+        <f t="shared" si="8"/>
+        <v>135</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J12">
-        <f t="shared" si="8"/>
-        <v>2.1739130434782608</v>
+        <f t="shared" si="5"/>
+        <v>2.1459227467811157</v>
       </c>
       <c r="K12">
-        <f t="shared" si="9"/>
-        <v>135.53387573964497</v>
+        <v>18</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.5751072961373391</v>
       </c>
       <c r="O12" s="35">
         <f t="shared" si="1"/>
-        <v>3.2608695652173912E-2</v>
+        <v>2.575107296137339E-2</v>
       </c>
       <c r="P12" s="35">
         <f t="shared" si="2"/>
-        <v>6.5217391304347824E-2</v>
+        <v>6.4377682403433473E-2</v>
       </c>
       <c r="Q12" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.7253218884120164E-2</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
@@ -48238,7 +48232,7 @@
         <v>12.695652173913043</v>
       </c>
       <c r="E13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
       <c r="F13">
@@ -48249,26 +48243,25 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="7"/>
-        <v>103</v>
+        <f t="shared" si="8"/>
+        <v>150</v>
       </c>
       <c r="I13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J13">
-        <f t="shared" si="8"/>
-        <v>2.7173913043478262</v>
+        <f t="shared" si="5"/>
+        <v>1.7167381974248928</v>
       </c>
       <c r="K13">
-        <f t="shared" si="9"/>
-        <v>150.59319526627218</v>
+        <v>20</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
-        <v>0.54347826086956519</v>
+        <f t="shared" si="6"/>
+        <v>1.2875536480686696</v>
       </c>
       <c r="O13" s="35">
         <f t="shared" si="1"/>
@@ -48276,11 +48269,11 @@
       </c>
       <c r="P13" s="35">
         <f t="shared" si="2"/>
-        <v>8.1521739130434784E-2</v>
+        <v>5.1502145922746781E-2</v>
       </c>
       <c r="Q13" s="35">
         <f t="shared" si="3"/>
-        <v>1.6304347826086956E-2</v>
+        <v>3.8626609442060082E-2</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -48295,49 +48288,48 @@
         <v>12.888888888888889</v>
       </c>
       <c r="E14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1100</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>1.6304347826086956</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="7"/>
-        <v>113</v>
+        <f t="shared" si="8"/>
+        <v>165</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <f t="shared" si="8"/>
-        <v>1.6304347826086956</v>
+        <f t="shared" si="5"/>
+        <v>0.85836909871244638</v>
       </c>
       <c r="K14">
-        <f t="shared" si="9"/>
-        <v>165.65251479289938</v>
+        <v>22</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.1459227467811157</v>
       </c>
       <c r="O14" s="35">
         <f t="shared" si="1"/>
-        <v>4.8913043478260872E-2</v>
+        <v>0</v>
       </c>
       <c r="P14" s="35">
         <f t="shared" si="2"/>
-        <v>4.8913043478260872E-2</v>
+        <v>2.575107296137339E-2</v>
       </c>
       <c r="Q14" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.4377682403433473E-2</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -48352,45 +48344,48 @@
         <v>13.80952380952381</v>
       </c>
       <c r="E15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1200</v>
       </c>
-      <c r="F15" t="e">
-        <v>#N/A</v>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>0.42918454935622319</v>
       </c>
       <c r="H15">
-        <f t="shared" si="7"/>
-        <v>123</v>
+        <f t="shared" si="8"/>
+        <v>180</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15">
-        <f t="shared" si="8"/>
-        <v>1.0869565217391304</v>
+        <f t="shared" si="5"/>
+        <v>0.85836909871244638</v>
       </c>
       <c r="K15">
-        <f t="shared" si="9"/>
-        <v>180.71183431952659</v>
+        <v>24</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M15">
-        <f t="shared" si="5"/>
-        <v>0.54347826086956519</v>
+        <f t="shared" si="6"/>
+        <v>1.2875536480686696</v>
       </c>
       <c r="O15" s="35">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2875536480686695E-2</v>
       </c>
       <c r="P15" s="35">
         <f t="shared" si="2"/>
-        <v>3.2608695652173912E-2</v>
+        <v>2.575107296137339E-2</v>
       </c>
       <c r="Q15" s="35">
         <f t="shared" si="3"/>
-        <v>1.6304347826086956E-2</v>
+        <v>3.8626609442060082E-2</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
@@ -48405,33 +48400,8 @@
         <v>31.25</v>
       </c>
       <c r="E16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1300</v>
-      </c>
-      <c r="F16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="7"/>
-        <v>133</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="8"/>
-        <v>0.54347826086956519</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="9"/>
-        <v>195.77115384615379</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="5"/>
-        <v>0.54347826086956519</v>
       </c>
       <c r="O16" s="35">
         <f t="shared" si="1"/>
@@ -48439,14 +48409,14 @@
       </c>
       <c r="P16" s="35">
         <f t="shared" si="2"/>
-        <v>1.6304347826086956E-2</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="35">
         <f t="shared" si="3"/>
-        <v>1.6304347826086956E-2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="29">
         <v>149</v>
       </c>
@@ -48458,7 +48428,7 @@
         <v>37.25</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="29">
         <v>166</v>
       </c>
@@ -48470,7 +48440,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="29">
         <v>146</v>
       </c>
@@ -48482,7 +48452,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="29">
         <v>291</v>
       </c>
@@ -48493,23 +48463,8 @@
         <f t="shared" si="0"/>
         <v>10.777777777777779</v>
       </c>
-      <c r="G20" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" t="s">
-        <v>93</v>
-      </c>
-      <c r="M20" t="s">
-        <v>94</v>
-      </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="29">
         <v>277</v>
       </c>
@@ -48520,31 +48475,8 @@
         <f t="shared" si="0"/>
         <v>9.5517241379310338</v>
       </c>
-      <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21">
-        <f>MAX($C$1:$C$184)</f>
-        <v>170</v>
-      </c>
-      <c r="H21">
-        <f>MIN($C$1:$C$184)</f>
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <f>AVERAGE($C$1:$C$184)</f>
-        <v>33.745108695652178</v>
-      </c>
-      <c r="K21">
-        <f>_xlfn.STDEV.P($C$1:$C$184)</f>
-        <v>30.007205257729179</v>
-      </c>
-      <c r="M21">
-        <f>G21-H21</f>
-        <v>169</v>
-      </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="29">
         <v>247</v>
       </c>
@@ -48555,31 +48487,8 @@
         <f t="shared" si="0"/>
         <v>15.4375</v>
       </c>
-      <c r="F22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22">
-        <f>MAX($B1:$B184)</f>
-        <v>1450</v>
-      </c>
-      <c r="H22">
-        <f>MIN($B1:$B184)</f>
-        <v>20</v>
-      </c>
-      <c r="I22">
-        <f>AVERAGE($B1:$B184)</f>
-        <v>299.62717391304346</v>
-      </c>
-      <c r="K22">
-        <f>_xlfn.STDEV.P(B1:$B184)</f>
-        <v>199.65770142881874</v>
-      </c>
-      <c r="M22">
-        <f>G22-H22</f>
-        <v>1430</v>
-      </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="29">
         <v>213</v>
       </c>
@@ -48590,27 +48499,8 @@
         <f t="shared" si="0"/>
         <v>23.666666666666668</v>
       </c>
-      <c r="F23" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23">
-        <f>MAX($D2:$D185)</f>
-        <v>185</v>
-      </c>
-      <c r="H23">
-        <f>MIN($D2:$D185)</f>
-        <v>3.2124999999999999</v>
-      </c>
-      <c r="I23">
-        <f>AVERAGE($D1:$D185)</f>
-        <v>18.41219962516373</v>
-      </c>
-      <c r="K23">
-        <f>_xlfn.STDEV.P(D2:$D185)</f>
-        <v>26.052309568263947</v>
-      </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="29">
         <v>557</v>
       </c>
@@ -48622,7 +48512,7 @@
         <v>5.9572192513368982</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="29">
         <v>607</v>
       </c>
@@ -48634,7 +48524,7 @@
         <v>5.7809523809523808</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="29">
         <v>312</v>
       </c>
@@ -48645,18 +48535,8 @@
         <f t="shared" si="0"/>
         <v>11.142857142857142</v>
       </c>
-      <c r="G26">
-        <v>100</v>
-      </c>
-      <c r="H26">
-        <v>18</v>
-      </c>
-      <c r="K26">
-        <f>G26/H26</f>
-        <v>5.5555555555555554</v>
-      </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="29">
         <v>204</v>
       </c>
@@ -48667,18 +48547,8 @@
         <f t="shared" si="0"/>
         <v>14.571428571428571</v>
       </c>
-      <c r="G27">
-        <v>300</v>
-      </c>
-      <c r="H27">
-        <v>35</v>
-      </c>
-      <c r="K27">
-        <f t="shared" ref="K27" si="11">G27/H27</f>
-        <v>8.5714285714285712</v>
-      </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="29">
         <v>305</v>
       </c>
@@ -48689,18 +48559,8 @@
         <f t="shared" si="0"/>
         <v>8.026315789473685</v>
       </c>
-      <c r="G28">
-        <v>500</v>
-      </c>
-      <c r="H28">
-        <v>70</v>
-      </c>
-      <c r="K28">
-        <f>G28/H28</f>
-        <v>7.1428571428571432</v>
-      </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="29">
         <v>230</v>
       </c>
@@ -48712,7 +48572,7 @@
         <v>12.777777777777779</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="29">
         <v>387</v>
       </c>
@@ -48724,7 +48584,7 @@
         <v>16.125</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="29">
         <v>217</v>
       </c>
@@ -48736,7 +48596,7 @@
         <v>27.125</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="29">
         <v>116</v>
       </c>
@@ -48748,7 +48608,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B33" s="29">
         <v>166</v>
       </c>
@@ -48759,11 +48619,8 @@
         <f t="shared" si="0"/>
         <v>166</v>
       </c>
-      <c r="L33" t="s">
-        <v>95</v>
-      </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="29">
         <v>275</v>
       </c>
@@ -48774,12 +48631,8 @@
         <f t="shared" si="0"/>
         <v>39.285714285714285</v>
       </c>
-      <c r="L34">
-        <f>MEDIAN($C$1:$C$184)</f>
-        <v>24.5</v>
-      </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="29">
         <v>216</v>
       </c>
@@ -48790,12 +48643,8 @@
         <f t="shared" si="0"/>
         <v>21.6</v>
       </c>
-      <c r="L35">
-        <f>MEDIAN($B1:$B184)</f>
-        <v>267.5</v>
-      </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="29">
         <v>536</v>
       </c>
@@ -48807,7 +48656,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="29">
         <v>320</v>
       </c>
@@ -48819,7 +48668,7 @@
         <v>35.555555555555557</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="29">
         <v>373</v>
       </c>
@@ -48831,7 +48680,7 @@
         <v>28.692307692307693</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="29">
         <v>282</v>
       </c>
@@ -48843,7 +48692,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="29">
         <v>320</v>
       </c>
@@ -48855,7 +48704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="29">
         <v>370</v>
       </c>
@@ -48867,7 +48716,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="29">
         <v>282</v>
       </c>
@@ -48879,7 +48728,7 @@
         <v>56.4</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="29">
         <v>245</v>
       </c>
@@ -48891,7 +48740,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" s="29">
         <v>100</v>
       </c>
@@ -48903,7 +48752,7 @@
         <v>5.2631578947368425</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" s="29">
         <v>200</v>
       </c>
@@ -48915,7 +48764,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B46" s="29">
         <v>361</v>
       </c>
@@ -48927,7 +48776,7 @@
         <v>12.033333333333333</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" s="29">
         <v>393</v>
       </c>
@@ -48938,8 +48787,23 @@
         <f t="shared" si="0"/>
         <v>6.55</v>
       </c>
+      <c r="H47" t="s">
+        <v>90</v>
+      </c>
+      <c r="I47" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" t="s">
+        <v>92</v>
+      </c>
+      <c r="L47" t="s">
+        <v>93</v>
+      </c>
+      <c r="N47" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B48" s="29">
         <v>245</v>
       </c>
@@ -48950,8 +48814,31 @@
         <f t="shared" si="0"/>
         <v>11.666666666666666</v>
       </c>
+      <c r="G48" t="s">
+        <v>76</v>
+      </c>
+      <c r="H48">
+        <f>MAX($C$1:$C$184)</f>
+        <v>170</v>
+      </c>
+      <c r="I48">
+        <f>MIN($C$1:$C$184)</f>
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <f>AVERAGE($C$1:$C$184)</f>
+        <v>33.745108695652178</v>
+      </c>
+      <c r="L48">
+        <f>_xlfn.STDEV.P($C$1:$C$184)</f>
+        <v>30.007205257729179</v>
+      </c>
+      <c r="N48">
+        <f>H48-I48</f>
+        <v>169</v>
+      </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B49" s="29">
         <v>323</v>
       </c>
@@ -48962,8 +48849,31 @@
         <f t="shared" si="0"/>
         <v>10.766666666666667</v>
       </c>
+      <c r="G49" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49">
+        <f>MAX($B1:$B184)</f>
+        <v>1450</v>
+      </c>
+      <c r="I49">
+        <f>MIN($B1:$B184)</f>
+        <v>20</v>
+      </c>
+      <c r="J49">
+        <f>AVERAGE($B1:$B184)</f>
+        <v>299.62717391304346</v>
+      </c>
+      <c r="L49">
+        <f>_xlfn.STDEV.P(B1:$B184)</f>
+        <v>199.65770142881874</v>
+      </c>
+      <c r="N49">
+        <f>H49-I49</f>
+        <v>1430</v>
+      </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B50" s="29">
         <v>290</v>
       </c>
@@ -48974,8 +48884,27 @@
         <f t="shared" si="0"/>
         <v>22.307692307692307</v>
       </c>
+      <c r="G50" t="s">
+        <v>104</v>
+      </c>
+      <c r="H50">
+        <f>MAX($D2:$D185)</f>
+        <v>185</v>
+      </c>
+      <c r="I50">
+        <f>MIN($D2:$D185)</f>
+        <v>3.2124999999999999</v>
+      </c>
+      <c r="J50">
+        <f>AVERAGE($D1:$D185)</f>
+        <v>18.41219962516373</v>
+      </c>
+      <c r="L50">
+        <f>_xlfn.STDEV.P(D2:$D185)</f>
+        <v>26.052309568263947</v>
+      </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B51" s="29">
         <v>161</v>
       </c>
@@ -48987,7 +48916,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B52" s="29">
         <v>182</v>
       </c>
@@ -48999,7 +48928,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B53" s="30">
         <v>400</v>
       </c>
@@ -49010,8 +48939,18 @@
         <f t="shared" si="0"/>
         <v>12.121212121212121</v>
       </c>
+      <c r="H53">
+        <v>100</v>
+      </c>
+      <c r="I53">
+        <v>18</v>
+      </c>
+      <c r="L53">
+        <f>H53/I53</f>
+        <v>5.5555555555555554</v>
+      </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B54" s="30">
         <v>525</v>
       </c>
@@ -49022,8 +48961,18 @@
         <f t="shared" si="0"/>
         <v>4.0384615384615383</v>
       </c>
+      <c r="H54">
+        <v>300</v>
+      </c>
+      <c r="I54">
+        <v>35</v>
+      </c>
+      <c r="L54">
+        <f t="shared" ref="L54" si="10">H54/I54</f>
+        <v>8.5714285714285712</v>
+      </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B55" s="30">
         <v>250</v>
       </c>
@@ -49034,8 +48983,18 @@
         <f t="shared" si="0"/>
         <v>83.333333333333329</v>
       </c>
+      <c r="H55">
+        <v>500</v>
+      </c>
+      <c r="I55">
+        <v>70</v>
+      </c>
+      <c r="L55">
+        <f>H55/I55</f>
+        <v>7.1428571428571432</v>
+      </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" s="30">
         <v>368</v>
       </c>
@@ -49047,7 +49006,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B57" s="30">
         <v>456</v>
       </c>
@@ -49059,7 +49018,7 @@
         <v>27.636363636363637</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B58" s="30">
         <v>211</v>
       </c>
@@ -49071,7 +49030,7 @@
         <v>105.5</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B59" s="30">
         <v>278</v>
       </c>
@@ -49083,7 +49042,7 @@
         <v>12.636363636363637</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B60" s="30">
         <v>196</v>
       </c>
@@ -49094,8 +49053,11 @@
         <f t="shared" si="0"/>
         <v>12.25</v>
       </c>
+      <c r="M60" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B61" s="30">
         <v>164</v>
       </c>
@@ -49106,8 +49068,12 @@
         <f t="shared" si="0"/>
         <v>8.6315789473684212</v>
       </c>
+      <c r="M61">
+        <f>MEDIAN($C$1:$C$184)</f>
+        <v>24.5</v>
+      </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B62" s="30">
         <v>244</v>
       </c>
@@ -49118,8 +49084,12 @@
         <f t="shared" si="0"/>
         <v>11.619047619047619</v>
       </c>
+      <c r="M62">
+        <f>MEDIAN($B1:$B184)</f>
+        <v>267.5</v>
+      </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B63" s="30">
         <v>20</v>
       </c>
@@ -49131,7 +49101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B64" s="30">
         <v>407</v>
       </c>
@@ -49163,7 +49133,7 @@
         <v>100</v>
       </c>
       <c r="D66" s="29">
-        <f t="shared" ref="D66:D129" si="12">B66/C66</f>
+        <f t="shared" ref="D66:D129" si="11">B66/C66</f>
         <v>5.69</v>
       </c>
     </row>
@@ -49175,7 +49145,7 @@
         <v>84</v>
       </c>
       <c r="D67" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9.2142857142857135</v>
       </c>
     </row>
@@ -49187,7 +49157,7 @@
         <v>2</v>
       </c>
       <c r="D68" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>139.5</v>
       </c>
     </row>
@@ -49199,7 +49169,7 @@
         <v>3</v>
       </c>
       <c r="D69" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>102.33333333333333</v>
       </c>
     </row>
@@ -49211,7 +49181,7 @@
         <v>5</v>
       </c>
       <c r="D70" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>52.8</v>
       </c>
     </row>
@@ -49223,7 +49193,7 @@
         <v>7</v>
       </c>
       <c r="D71" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>38</v>
       </c>
     </row>
@@ -49235,7 +49205,7 @@
         <v>75</v>
       </c>
       <c r="D72" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.3733333333333331</v>
       </c>
     </row>
@@ -49247,7 +49217,7 @@
         <v>86</v>
       </c>
       <c r="D73" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4.5348837209302326</v>
       </c>
     </row>
@@ -49259,7 +49229,7 @@
         <v>116</v>
       </c>
       <c r="D74" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.2241379310344831</v>
       </c>
     </row>
@@ -49271,7 +49241,7 @@
         <v>72</v>
       </c>
       <c r="D75" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.666666666666667</v>
       </c>
     </row>
@@ -49283,7 +49253,7 @@
         <v>50</v>
       </c>
       <c r="D76" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8.94</v>
       </c>
     </row>
@@ -49295,7 +49265,7 @@
         <v>103</v>
       </c>
       <c r="D77" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8.1941747572815533</v>
       </c>
     </row>
@@ -49307,7 +49277,7 @@
         <v>53</v>
       </c>
       <c r="D78" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>14.283018867924529</v>
       </c>
     </row>
@@ -49319,7 +49289,7 @@
         <v>27</v>
       </c>
       <c r="D79" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>14.703703703703704</v>
       </c>
     </row>
@@ -49331,7 +49301,7 @@
         <v>11</v>
       </c>
       <c r="D80" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>22.818181818181817</v>
       </c>
     </row>
@@ -49343,7 +49313,7 @@
         <v>29</v>
       </c>
       <c r="D81" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>10.862068965517242</v>
       </c>
     </row>
@@ -49355,7 +49325,7 @@
         <v>16</v>
       </c>
       <c r="D82" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>20.25</v>
       </c>
     </row>
@@ -49367,7 +49337,7 @@
         <v>30</v>
       </c>
       <c r="D83" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>14.766666666666667</v>
       </c>
     </row>
@@ -49379,7 +49349,7 @@
         <v>17</v>
       </c>
       <c r="D84" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>17.941176470588236</v>
       </c>
     </row>
@@ -49391,7 +49361,7 @@
         <v>16</v>
       </c>
       <c r="D85" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
     </row>
@@ -49403,7 +49373,7 @@
         <v>71</v>
       </c>
       <c r="D86" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.6901408450704229</v>
       </c>
     </row>
@@ -49415,7 +49385,7 @@
         <v>78</v>
       </c>
       <c r="D87" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4.8717948717948714</v>
       </c>
     </row>
@@ -49427,7 +49397,7 @@
         <v>44</v>
       </c>
       <c r="D88" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>6.1590909090909092</v>
       </c>
     </row>
@@ -49439,7 +49409,7 @@
         <v>24</v>
       </c>
       <c r="D89" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9.0416666666666661</v>
       </c>
     </row>
@@ -49451,7 +49421,7 @@
         <v>15</v>
       </c>
       <c r="D90" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>16.133333333333333</v>
       </c>
     </row>
@@ -49463,7 +49433,7 @@
         <v>18</v>
       </c>
       <c r="D91" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>15.055555555555555</v>
       </c>
     </row>
@@ -49475,7 +49445,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>27.90909090909091</v>
       </c>
     </row>
@@ -49487,7 +49457,7 @@
         <v>48</v>
       </c>
       <c r="D93" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.666666666666667</v>
       </c>
     </row>
@@ -49499,7 +49469,7 @@
         <v>43</v>
       </c>
       <c r="D94" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.6279069767441863</v>
       </c>
     </row>
@@ -49511,7 +49481,7 @@
         <v>32</v>
       </c>
       <c r="D95" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9.125</v>
       </c>
     </row>
@@ -49523,7 +49493,7 @@
         <v>27</v>
       </c>
       <c r="D96" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>10.222222222222221</v>
       </c>
     </row>
@@ -49535,7 +49505,7 @@
         <v>10</v>
       </c>
       <c r="D97" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>29.4</v>
       </c>
     </row>
@@ -49547,7 +49517,7 @@
         <v>32</v>
       </c>
       <c r="D98" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>12.5625</v>
       </c>
     </row>
@@ -49559,7 +49529,7 @@
         <v>61</v>
       </c>
       <c r="D99" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.4754098360655741</v>
       </c>
     </row>
@@ -49571,7 +49541,7 @@
         <v>49</v>
       </c>
       <c r="D100" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9.2857142857142865</v>
       </c>
     </row>
@@ -49583,7 +49553,7 @@
         <v>28</v>
       </c>
       <c r="D101" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>13.5</v>
       </c>
     </row>
@@ -49595,7 +49565,7 @@
         <v>25</v>
       </c>
       <c r="D102" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>16.96</v>
       </c>
     </row>
@@ -49607,7 +49577,7 @@
         <v>13</v>
       </c>
       <c r="D103" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>11.923076923076923</v>
       </c>
     </row>
@@ -49619,7 +49589,7 @@
         <v>170</v>
       </c>
       <c r="D104" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>7.2352941176470589</v>
       </c>
     </row>
@@ -49631,7 +49601,7 @@
         <v>71</v>
       </c>
       <c r="D105" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9.2676056338028161</v>
       </c>
     </row>
@@ -49643,7 +49613,7 @@
         <v>108</v>
       </c>
       <c r="D106" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>6.166666666666667</v>
       </c>
     </row>
@@ -49655,7 +49625,7 @@
         <v>25</v>
       </c>
       <c r="D107" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
     </row>
@@ -49667,7 +49637,7 @@
         <v>25</v>
       </c>
       <c r="D108" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>20.52</v>
       </c>
     </row>
@@ -49679,7 +49649,7 @@
         <v>25</v>
       </c>
       <c r="D109" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>20.28</v>
       </c>
     </row>
@@ -49691,7 +49661,7 @@
         <v>29</v>
       </c>
       <c r="D110" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
     </row>
@@ -49703,7 +49673,7 @@
         <v>56</v>
       </c>
       <c r="D111" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.1964285714285712</v>
       </c>
     </row>
@@ -49715,7 +49685,7 @@
         <v>59</v>
       </c>
       <c r="D112" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8.5084745762711869</v>
       </c>
     </row>
@@ -49727,7 +49697,7 @@
         <v>46</v>
       </c>
       <c r="D113" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8.4347826086956523</v>
       </c>
     </row>
@@ -49739,7 +49709,7 @@
         <v>65</v>
       </c>
       <c r="D114" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>6.7692307692307692</v>
       </c>
     </row>
@@ -49751,7 +49721,7 @@
         <v>93</v>
       </c>
       <c r="D115" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>15.591397849462366</v>
       </c>
     </row>
@@ -49763,7 +49733,7 @@
         <v>99</v>
       </c>
       <c r="D116" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>11.818181818181818</v>
       </c>
     </row>
@@ -49775,7 +49745,7 @@
         <v>10</v>
       </c>
       <c r="D117" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>31.9</v>
       </c>
     </row>
@@ -49787,7 +49757,7 @@
         <v>60</v>
       </c>
       <c r="D118" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4.833333333333333</v>
       </c>
     </row>
@@ -49799,7 +49769,7 @@
         <v>37</v>
       </c>
       <c r="D119" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.1891891891891895</v>
       </c>
     </row>
@@ -49811,7 +49781,7 @@
         <v>9</v>
       </c>
       <c r="D120" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>28.888888888888889</v>
       </c>
     </row>
@@ -49823,7 +49793,7 @@
         <v>13</v>
       </c>
       <c r="D121" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>14.23076923076923</v>
       </c>
     </row>
@@ -49835,7 +49805,7 @@
         <v>59</v>
       </c>
       <c r="D122" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4.8305084745762707</v>
       </c>
     </row>
@@ -49847,7 +49817,7 @@
         <v>21</v>
       </c>
       <c r="D123" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8.6190476190476186</v>
       </c>
     </row>
@@ -49859,7 +49829,7 @@
         <v>36</v>
       </c>
       <c r="D124" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4.7777777777777777</v>
       </c>
     </row>
@@ -49871,7 +49841,7 @@
         <v>32</v>
       </c>
       <c r="D125" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>4.1875</v>
       </c>
     </row>
@@ -49883,7 +49853,7 @@
         <v>22</v>
       </c>
       <c r="D126" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.6363636363636367</v>
       </c>
     </row>
@@ -49895,7 +49865,7 @@
         <v>22</v>
       </c>
       <c r="D127" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>9.3181818181818183</v>
       </c>
     </row>
@@ -49907,7 +49877,7 @@
         <v>48</v>
       </c>
       <c r="D128" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.583333333333333</v>
       </c>
     </row>
@@ -49919,7 +49889,7 @@
         <v>69</v>
       </c>
       <c r="D129" s="29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>6.5507246376811592</v>
       </c>
     </row>
@@ -49931,7 +49901,7 @@
         <v>33</v>
       </c>
       <c r="D130" s="29">
-        <f t="shared" ref="D130:D184" si="13">B130/C130</f>
+        <f t="shared" ref="D130:D184" si="12">B130/C130</f>
         <v>8.6666666666666661</v>
       </c>
     </row>
@@ -49943,7 +49913,7 @@
         <v>118</v>
       </c>
       <c r="D131" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.9322033898305087</v>
       </c>
     </row>
@@ -49955,7 +49925,7 @@
         <v>102</v>
       </c>
       <c r="D132" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.8627450980392153</v>
       </c>
     </row>
@@ -49967,7 +49937,7 @@
         <v>29</v>
       </c>
       <c r="D133" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>10.482758620689655</v>
       </c>
     </row>
@@ -49979,7 +49949,7 @@
         <v>36</v>
       </c>
       <c r="D134" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.3888888888888893</v>
       </c>
     </row>
@@ -49991,7 +49961,7 @@
         <v>35</v>
       </c>
       <c r="D135" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.9714285714285715</v>
       </c>
     </row>
@@ -50003,7 +49973,7 @@
         <v>34</v>
       </c>
       <c r="D136" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>6.2647058823529411</v>
       </c>
     </row>
@@ -50015,7 +49985,7 @@
         <v>23</v>
       </c>
       <c r="D137" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.4782608695652177</v>
       </c>
     </row>
@@ -50027,7 +49997,7 @@
         <v>14</v>
       </c>
       <c r="D138" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7.9285714285714288</v>
       </c>
     </row>
@@ -50039,7 +50009,7 @@
         <v>41</v>
       </c>
       <c r="D139" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.8780487804878048</v>
       </c>
     </row>
@@ -50051,7 +50021,7 @@
         <v>15</v>
       </c>
       <c r="D140" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9.4666666666666668</v>
       </c>
     </row>
@@ -50063,7 +50033,7 @@
         <v>60</v>
       </c>
       <c r="D141" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.4666666666666668</v>
       </c>
     </row>
@@ -50075,7 +50045,7 @@
         <v>43</v>
       </c>
       <c r="D142" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.9534883720930232</v>
       </c>
     </row>
@@ -50087,7 +50057,7 @@
         <v>38</v>
       </c>
       <c r="D143" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.1842105263157894</v>
       </c>
     </row>
@@ -50099,7 +50069,7 @@
         <v>19</v>
       </c>
       <c r="D144" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>10.210526315789474</v>
       </c>
     </row>
@@ -50111,7 +50081,7 @@
         <v>10</v>
       </c>
       <c r="D145" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -50123,7 +50093,7 @@
         <v>29</v>
       </c>
       <c r="D146" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>6.3103448275862073</v>
       </c>
     </row>
@@ -50135,7 +50105,7 @@
         <v>9</v>
       </c>
       <c r="D147" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9.8888888888888893</v>
       </c>
     </row>
@@ -50147,7 +50117,7 @@
         <v>9</v>
       </c>
       <c r="D148" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
     </row>
@@ -50159,7 +50129,7 @@
         <v>20</v>
       </c>
       <c r="D149" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.8499999999999996</v>
       </c>
     </row>
@@ -50171,7 +50141,7 @@
         <v>22</v>
       </c>
       <c r="D150" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.4545454545454541</v>
       </c>
     </row>
@@ -50183,7 +50153,7 @@
         <v>12</v>
       </c>
       <c r="D151" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9.4166666666666661</v>
       </c>
     </row>
@@ -50195,7 +50165,7 @@
         <v>9</v>
       </c>
       <c r="D152" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9.1111111111111107</v>
       </c>
     </row>
@@ -50207,7 +50177,7 @@
         <v>18</v>
       </c>
       <c r="D153" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.0555555555555554</v>
       </c>
     </row>
@@ -50219,7 +50189,7 @@
         <v>14</v>
       </c>
       <c r="D154" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>8.2142857142857135</v>
       </c>
     </row>
@@ -50231,7 +50201,7 @@
         <v>19</v>
       </c>
       <c r="D155" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
     </row>
@@ -50243,7 +50213,7 @@
         <v>28</v>
       </c>
       <c r="D156" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.7857142857142856</v>
       </c>
     </row>
@@ -50255,7 +50225,7 @@
         <v>7</v>
       </c>
       <c r="D157" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>19.857142857142858</v>
       </c>
     </row>
@@ -50267,7 +50237,7 @@
         <v>36</v>
       </c>
       <c r="D158" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.1944444444444446</v>
       </c>
     </row>
@@ -50279,7 +50249,7 @@
         <v>12</v>
       </c>
       <c r="D159" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>8.0833333333333339</v>
       </c>
     </row>
@@ -50291,7 +50261,7 @@
         <v>62</v>
       </c>
       <c r="D160" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.838709677419355</v>
       </c>
     </row>
@@ -50303,7 +50273,7 @@
         <v>41</v>
       </c>
       <c r="D161" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7.0975609756097562</v>
       </c>
     </row>
@@ -50315,7 +50285,7 @@
         <v>37</v>
       </c>
       <c r="D162" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.3243243243243246</v>
       </c>
     </row>
@@ -50327,7 +50297,7 @@
         <v>41</v>
       </c>
       <c r="D163" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.4146341463414633</v>
       </c>
     </row>
@@ -50339,7 +50309,7 @@
         <v>14.1</v>
       </c>
       <c r="D164" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7.2340425531914896</v>
       </c>
     </row>
@@ -50351,7 +50321,7 @@
         <v>7</v>
       </c>
       <c r="D165" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>18.571428571428573</v>
       </c>
     </row>
@@ -50363,7 +50333,7 @@
         <v>5</v>
       </c>
       <c r="D166" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>24.4</v>
       </c>
     </row>
@@ -50375,7 +50345,7 @@
         <v>77</v>
       </c>
       <c r="D167" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.8441558441558441</v>
       </c>
     </row>
@@ -50387,7 +50357,7 @@
         <v>80</v>
       </c>
       <c r="D168" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.2124999999999999</v>
       </c>
     </row>
@@ -50399,7 +50369,7 @@
         <v>70</v>
       </c>
       <c r="D169" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.3714285714285714</v>
       </c>
     </row>
@@ -50411,7 +50381,7 @@
         <v>63</v>
       </c>
       <c r="D170" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
@@ -50423,7 +50393,7 @@
         <v>62</v>
       </c>
       <c r="D171" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.2419354838709675</v>
       </c>
     </row>
@@ -50435,7 +50405,7 @@
         <v>34</v>
       </c>
       <c r="D172" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.5882352941176467</v>
       </c>
     </row>
@@ -50447,7 +50417,7 @@
         <v>40</v>
       </c>
       <c r="D173" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.875</v>
       </c>
     </row>
@@ -50459,7 +50429,7 @@
         <v>30</v>
       </c>
       <c r="D174" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.2666666666666666</v>
       </c>
     </row>
@@ -50471,7 +50441,7 @@
         <v>19</v>
       </c>
       <c r="D175" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.7368421052631575</v>
       </c>
     </row>
@@ -50483,7 +50453,7 @@
         <v>40</v>
       </c>
       <c r="D176" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.25</v>
       </c>
     </row>
@@ -50495,7 +50465,7 @@
         <v>53</v>
       </c>
       <c r="D177" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
     </row>
@@ -50507,7 +50477,7 @@
         <v>24</v>
       </c>
       <c r="D178" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.458333333333333</v>
       </c>
     </row>
@@ -50519,7 +50489,7 @@
         <v>37</v>
       </c>
       <c r="D179" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.3243243243243246</v>
       </c>
     </row>
@@ -50531,7 +50501,7 @@
         <v>20</v>
       </c>
       <c r="D180" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>7.3</v>
       </c>
     </row>
@@ -50543,7 +50513,7 @@
         <v>18</v>
       </c>
       <c r="D181" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>6.166666666666667</v>
       </c>
     </row>
@@ -50555,7 +50525,7 @@
         <v>20</v>
       </c>
       <c r="D182" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.5</v>
       </c>
     </row>
@@ -50567,7 +50537,7 @@
         <v>64</v>
       </c>
       <c r="D183" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>6.03125</v>
       </c>
     </row>
@@ -50579,108 +50549,442 @@
         <v>41</v>
       </c>
       <c r="D184" s="29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9.5121951219512191</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B185" s="74">
+        <v>90.6</v>
+      </c>
+      <c r="C185" s="74">
+        <v>24</v>
+      </c>
       <c r="D185" s="29"/>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B186" s="73">
+        <v>112</v>
+      </c>
+      <c r="C186" s="73">
+        <v>30</v>
+      </c>
       <c r="D186" s="29"/>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B187" s="73">
+        <v>80</v>
+      </c>
+      <c r="C187" s="73">
+        <v>27</v>
+      </c>
       <c r="D187" s="29"/>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B188" s="73">
+        <v>123</v>
+      </c>
+      <c r="C188" s="73">
+        <v>28</v>
+      </c>
       <c r="D188" s="29"/>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B189" s="73">
+        <v>93</v>
+      </c>
+      <c r="C189" s="73">
+        <v>29</v>
+      </c>
       <c r="D189" s="29"/>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B190" s="73">
+        <v>86</v>
+      </c>
+      <c r="C190" s="73">
+        <v>28</v>
+      </c>
       <c r="D190" s="29"/>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B191" s="73">
+        <v>243</v>
+      </c>
+      <c r="C191" s="73">
+        <v>65</v>
+      </c>
       <c r="D191" s="29"/>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B192" s="74">
+        <v>268</v>
+      </c>
+      <c r="C192" s="74">
+        <v>70</v>
+      </c>
       <c r="D192" s="29"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B193" s="73">
+        <v>288</v>
+      </c>
+      <c r="C193" s="73">
+        <v>60</v>
+      </c>
       <c r="D193" s="29"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B194" s="73">
+        <v>258</v>
+      </c>
+      <c r="C194" s="73">
+        <v>61</v>
+      </c>
       <c r="D194" s="29"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B195" s="73">
+        <v>172</v>
+      </c>
+      <c r="C195" s="73">
+        <v>38</v>
+      </c>
       <c r="D195" s="29"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B196" s="73">
+        <v>152</v>
+      </c>
+      <c r="C196" s="73">
+        <v>45</v>
+      </c>
       <c r="D196" s="29"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B197" s="73">
+        <v>183</v>
+      </c>
+      <c r="C197" s="73">
+        <v>46</v>
+      </c>
       <c r="D197" s="29"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B198" s="73">
+        <v>177</v>
+      </c>
+      <c r="C198" s="73">
+        <v>38</v>
+      </c>
       <c r="D198" s="29"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B199" s="73">
+        <v>213</v>
+      </c>
+      <c r="C199" s="73">
+        <v>58</v>
+      </c>
       <c r="D199" s="29"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B200" s="73">
+        <v>259</v>
+      </c>
+      <c r="C200" s="73">
+        <v>77</v>
+      </c>
       <c r="D200" s="29"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B201" s="73">
+        <v>222</v>
+      </c>
+      <c r="C201" s="73">
+        <v>72</v>
+      </c>
       <c r="D201" s="29"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B202" s="73">
+        <v>133</v>
+      </c>
+      <c r="C202" s="73">
+        <v>46</v>
+      </c>
       <c r="D202" s="29"/>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B203" s="73">
+        <v>70</v>
+      </c>
+      <c r="C203" s="73">
+        <v>17</v>
+      </c>
       <c r="D203" s="29"/>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B204" s="73">
+        <v>425</v>
+      </c>
+      <c r="C204" s="73">
+        <v>143</v>
+      </c>
       <c r="D204" s="29"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B205" s="73">
+        <v>429</v>
+      </c>
+      <c r="C205" s="73">
+        <v>115</v>
+      </c>
       <c r="D205" s="29"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B206" s="73">
+        <v>278</v>
+      </c>
+      <c r="C206" s="73">
+        <v>72</v>
+      </c>
       <c r="D206" s="29"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B207" s="73">
+        <v>427</v>
+      </c>
+      <c r="C207" s="73">
+        <v>114</v>
+      </c>
       <c r="D207" s="29"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B208" s="73">
+        <v>491</v>
+      </c>
+      <c r="C208" s="73">
+        <v>147</v>
+      </c>
       <c r="D208" s="29"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B209" s="73">
+        <v>469</v>
+      </c>
+      <c r="C209" s="73">
+        <v>130</v>
+      </c>
       <c r="D209" s="29"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B210" s="73">
+        <v>450</v>
+      </c>
+      <c r="C210" s="73">
+        <v>125</v>
+      </c>
       <c r="D210" s="29"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B211" s="73">
+        <v>398</v>
+      </c>
+      <c r="C211" s="73">
+        <v>77</v>
+      </c>
       <c r="D211" s="29"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B212" s="73">
+        <v>284</v>
+      </c>
+      <c r="C212" s="73">
+        <v>92</v>
+      </c>
       <c r="D212" s="29"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B213" s="73">
+        <v>480</v>
+      </c>
+      <c r="C213" s="73">
+        <v>126</v>
+      </c>
       <c r="D213" s="29"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B214" s="73">
+        <v>327</v>
+      </c>
+      <c r="C214" s="73">
+        <v>91</v>
+      </c>
       <c r="D214" s="29"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B215" s="73">
+        <v>494</v>
+      </c>
+      <c r="C215" s="73">
+        <v>168</v>
+      </c>
       <c r="D215" s="29"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B216" s="73">
+        <v>484</v>
+      </c>
+      <c r="C216" s="73">
+        <v>149</v>
+      </c>
       <c r="D216" s="29"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B217" s="73">
+        <v>669</v>
+      </c>
+      <c r="C217" s="73">
+        <v>188</v>
+      </c>
       <c r="D217" s="29"/>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B218" s="73">
+        <v>510</v>
+      </c>
+      <c r="C218" s="73">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B219" s="73">
+        <v>501</v>
+      </c>
+      <c r="C219" s="73">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B220" s="73">
+        <v>402</v>
+      </c>
+      <c r="C220" s="73">
+        <v>94.4</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B221" s="73">
+        <v>395</v>
+      </c>
+      <c r="C221" s="73">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B222" s="73">
+        <v>378</v>
+      </c>
+      <c r="C222" s="73">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B223" s="73">
+        <v>528</v>
+      </c>
+      <c r="C223" s="73">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B224" s="73">
+        <v>465</v>
+      </c>
+      <c r="C224" s="73">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B225" s="73">
+        <v>447</v>
+      </c>
+      <c r="C225" s="73">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B226" s="73">
+        <v>609</v>
+      </c>
+      <c r="C226" s="73">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B227" s="73">
+        <v>430</v>
+      </c>
+      <c r="C227" s="73">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B228" s="73">
+        <v>409</v>
+      </c>
+      <c r="C228" s="73">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B229" s="73">
+        <v>728</v>
+      </c>
+      <c r="C229" s="73">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B230" s="73">
+        <v>788</v>
+      </c>
+      <c r="C230" s="73">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B231" s="73">
+        <v>706</v>
+      </c>
+      <c r="C231" s="73">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B232" s="73">
+        <v>515</v>
+      </c>
+      <c r="C232" s="73">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="233" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B233" s="73">
+        <v>433</v>
+      </c>
+      <c r="C233" s="73">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="234" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B234" s="73">
+        <v>538</v>
+      </c>
+      <c r="C234" s="73">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -51608,7 +51912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C48:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
@@ -51660,7 +51964,7 @@
         <v>300</v>
       </c>
       <c r="Z55">
-        <f t="shared" ref="Z54:AB61" si="0">$Y55*Z$52</f>
+        <f t="shared" ref="Z55:AB61" si="0">$Y55*Z$52</f>
         <v>27</v>
       </c>
       <c r="AA55">

</xml_diff>

<commit_message>
added hood to charts
</commit_message>
<xml_diff>
--- a/channel database.xlsx
+++ b/channel database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24200" yWindow="2140" windowWidth="26580" windowHeight="23440" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="6740" yWindow="1180" windowWidth="35400" windowHeight="23440" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="channels" sheetId="1" r:id="rId1"/>
@@ -1797,11 +1797,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-763118112"/>
-        <c:axId val="-763303296"/>
+        <c:axId val="-2140328720"/>
+        <c:axId val="-2140325248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-763118112"/>
+        <c:axId val="-2140328720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.09"/>
@@ -1888,12 +1888,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763303296"/>
+        <c:crossAx val="-2140325248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763303296"/>
+        <c:axId val="-2140325248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -1980,7 +1980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763118112"/>
+        <c:crossAx val="-2140328720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2038,10 +2038,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.139975064998252"/>
+          <c:x val="0.101669802513465"/>
           <c:y val="0.0435111268939394"/>
-          <c:w val="0.803786243177084"/>
-          <c:h val="0.761806818181818"/>
+          <c:w val="0.855829658886894"/>
+          <c:h val="0.82395369011077"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2068,7 +2068,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="283A7F"/>
@@ -2210,7 +2210,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="2A8A6F"/>
@@ -2328,7 +2328,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="AD4A00"/>
@@ -2428,7 +2428,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="9C1F0A"/>
@@ -2552,7 +2552,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="4E67C8"/>
@@ -2662,8 +2662,73 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Hood</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>channels!$Q$33:$Q$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>644.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>972.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>336.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1187.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>965.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>channels!$R$33:$R$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:v>our topograpy</c:v>
           </c:tx>
@@ -2673,13 +2738,13 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
+            <c:symbol val="square"/>
+            <c:size val="11"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -2804,11 +2869,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-762851376"/>
-        <c:axId val="-762848256"/>
+        <c:axId val="-2079176784"/>
+        <c:axId val="-2079173024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-762851376"/>
+        <c:axId val="-2079176784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2823,7 +2888,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2837,7 +2902,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2890,12 +2955,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-762848256"/>
+        <c:crossAx val="-2079173024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-762848256"/>
+        <c:axId val="-2079173024"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2910,7 +2975,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2924,7 +2989,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2945,8 +3010,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0262992048167125"/>
-              <c:y val="0.260289535984848"/>
+              <c:x val="0.000762369838420108"/>
+              <c:y val="0.146184661239379"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2984,7 +3049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-762851376"/>
+        <c:crossAx val="-2079176784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3527,11 +3592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-323206928"/>
-        <c:axId val="-763185056"/>
+        <c:axId val="-2079134240"/>
+        <c:axId val="-2079130480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-323206928"/>
+        <c:axId val="-2079134240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -3619,12 +3684,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763185056"/>
+        <c:crossAx val="-2079130480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763185056"/>
+        <c:axId val="-2079130480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -3712,7 +3777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-323206928"/>
+        <c:crossAx val="-2079134240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4244,11 +4309,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-797752080"/>
-        <c:axId val="-797748960"/>
+        <c:axId val="-2078218672"/>
+        <c:axId val="-2078214912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-797752080"/>
+        <c:axId val="-2078218672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -4324,12 +4389,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797748960"/>
+        <c:crossAx val="-2078214912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-797748960"/>
+        <c:axId val="-2078214912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4405,7 +4470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797752080"/>
+        <c:crossAx val="-2078218672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4948,11 +5013,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-797764176"/>
-        <c:axId val="-519089088"/>
+        <c:axId val="-2078173600"/>
+        <c:axId val="-2078169840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-797764176"/>
+        <c:axId val="-2078173600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30000.0"/>
@@ -5034,12 +5099,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-519089088"/>
+        <c:crossAx val="-2078169840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-519089088"/>
+        <c:axId val="-2078169840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -5127,7 +5192,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797764176"/>
+        <c:crossAx val="-2078173600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5697,11 +5762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-797715952"/>
-        <c:axId val="-797759952"/>
+        <c:axId val="-2106472368"/>
+        <c:axId val="-2106459232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-797715952"/>
+        <c:axId val="-2106472368"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5783,12 +5848,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797759952"/>
+        <c:crossAx val="-2106459232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-797759952"/>
+        <c:axId val="-2106459232"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5878,7 +5943,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797715952"/>
+        <c:crossAx val="-2106472368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6480,11 +6545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-763078160"/>
-        <c:axId val="-763258032"/>
+        <c:axId val="-2078111824"/>
+        <c:axId val="-2078108064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-763078160"/>
+        <c:axId val="-2078111824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6553,12 +6618,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763258032"/>
+        <c:crossAx val="-2078108064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763258032"/>
+        <c:axId val="-2078108064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6634,7 +6699,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763078160"/>
+        <c:crossAx val="-2078111824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6902,11 +6967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-762879920"/>
-        <c:axId val="-762877872"/>
+        <c:axId val="-2078077664"/>
+        <c:axId val="-2078075184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-762879920"/>
+        <c:axId val="-2078077664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6943,12 +7008,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-762877872"/>
+        <c:crossAx val="-2078075184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-762877872"/>
+        <c:axId val="-2078075184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6994,7 +7059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-762879920"/>
+        <c:crossAx val="-2078077664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7269,11 +7334,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-322990528"/>
-        <c:axId val="-763344208"/>
+        <c:axId val="-2078049456"/>
+        <c:axId val="-2078046976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-322990528"/>
+        <c:axId val="-2078049456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7310,12 +7375,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763344208"/>
+        <c:crossAx val="-2078046976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763344208"/>
+        <c:axId val="-2078046976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7361,7 +7426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-322990528"/>
+        <c:crossAx val="-2078049456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8654,11 +8719,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-763272608"/>
-        <c:axId val="-763268928"/>
+        <c:axId val="-2078017360"/>
+        <c:axId val="-2078013600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-763272608"/>
+        <c:axId val="-2078017360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8699,6 +8764,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8761,12 +8827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763268928"/>
+        <c:crossAx val="-2078013600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763268928"/>
+        <c:axId val="-2078013600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8886,7 +8952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763272608"/>
+        <c:crossAx val="-2078017360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10229,11 +10295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-763018448"/>
-        <c:axId val="-763016016"/>
+        <c:axId val="-2077985152"/>
+        <c:axId val="-2077981392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-763018448"/>
+        <c:axId val="-2077985152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.0"/>
@@ -10342,12 +10408,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763016016"/>
+        <c:crossAx val="-2077981392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763016016"/>
+        <c:axId val="-2077981392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -10468,7 +10534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763018448"/>
+        <c:crossAx val="-2077985152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11083,11 +11149,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-763170256"/>
-        <c:axId val="-763136192"/>
+        <c:axId val="-2106499280"/>
+        <c:axId val="-2106495520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-763170256"/>
+        <c:axId val="-2106499280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.09"/>
@@ -11140,7 +11206,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -11175,12 +11240,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763136192"/>
+        <c:crossAx val="-2106495520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763136192"/>
+        <c:axId val="-2106495520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -11233,7 +11298,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -11268,7 +11332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763170256"/>
+        <c:crossAx val="-2106499280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11281,7 +11345,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11462,11 +11525,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-325016192"/>
-        <c:axId val="-799757104"/>
+        <c:axId val="-2140350848"/>
+        <c:axId val="-2140310160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-325016192"/>
+        <c:axId val="-2140350848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11479,7 +11542,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11493,7 +11556,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11546,7 +11609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-799757104"/>
+        <c:crossAx val="-2140310160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11554,7 +11617,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-799757104"/>
+        <c:axId val="-2140310160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11567,7 +11630,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11581,7 +11644,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11634,7 +11697,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-325016192"/>
+        <c:crossAx val="-2140350848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -11823,11 +11886,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-325052432"/>
-        <c:axId val="-325048976"/>
+        <c:axId val="-2140282928"/>
+        <c:axId val="-2140279168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-325052432"/>
+        <c:axId val="-2140282928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11840,7 +11903,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11854,7 +11917,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11907,7 +11970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-325048976"/>
+        <c:crossAx val="-2140279168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11915,7 +11978,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-325048976"/>
+        <c:axId val="-2140279168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11928,7 +11991,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11942,7 +12005,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -11995,7 +12058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-325052432"/>
+        <c:crossAx val="-2140282928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -12160,11 +12223,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-799833248"/>
-        <c:axId val="-799830128"/>
+        <c:axId val="-2140256912"/>
+        <c:axId val="-2140253152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-799833248"/>
+        <c:axId val="-2140256912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12244,7 +12307,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-799830128"/>
+        <c:crossAx val="-2140253152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12252,7 +12315,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-799830128"/>
+        <c:axId val="-2140253152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12329,7 +12392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-799833248"/>
+        <c:crossAx val="-2140256912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="15.0"/>
@@ -12539,11 +12602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-554757536"/>
-        <c:axId val="-554756176"/>
+        <c:axId val="-2140241808"/>
+        <c:axId val="-2140239328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-554757536"/>
+        <c:axId val="-2140241808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12600,12 +12663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-554756176"/>
+        <c:crossAx val="-2140239328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-554756176"/>
+        <c:axId val="-2140239328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12661,7 +12724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-554757536"/>
+        <c:crossAx val="-2140241808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12831,11 +12894,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="-1"/>
-        <c:axId val="-519166816"/>
-        <c:axId val="-797883872"/>
+        <c:axId val="-2140211776"/>
+        <c:axId val="-2140207744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-519166816"/>
+        <c:axId val="-2140211776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12928,7 +12991,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-797883872"/>
+        <c:crossAx val="-2140207744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12936,7 +12999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-797883872"/>
+        <c:axId val="-2140207744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13031,7 +13094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-519166816"/>
+        <c:crossAx val="-2140211776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15.0"/>
@@ -13095,10 +13158,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127895611377187"/>
+          <c:x val="0.11509826163564"/>
           <c:y val="0.0374701036407122"/>
-          <c:w val="0.820105561528687"/>
-          <c:h val="0.781911595358313"/>
+          <c:w val="0.840215726468166"/>
+          <c:h val="0.830344300026471"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -13125,7 +13188,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="283A7F"/>
@@ -13507,7 +13570,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="2A8A6F"/>
@@ -13739,7 +13802,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="AD4A00"/>
@@ -13917,7 +13980,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="9C1F0A"/>
@@ -14209,7 +14272,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="4E67C8"/>
@@ -14523,8 +14586,343 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Hood</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Width and Depths'!$U$2:$U$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>90.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>268.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>258.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>172.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>183.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>177.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>213.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>259.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>222.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>133.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>425.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>429.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>278.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>427.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>491.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>469.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>398.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>284.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>480.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>327.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>494.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>484.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>669.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>510.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>402.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>395.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>378.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>528.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>465.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>609.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>430.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>409.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>728.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>788.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>706.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>515.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>433.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>538.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Width and Depths'!$V$2:$V$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>143.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>115.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>147.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>151.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>94.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>86.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>127.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>92.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:v>Our Topography</c:v>
           </c:tx>
@@ -14534,13 +14932,13 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="9"/>
+            <c:symbol val="square"/>
+            <c:size val="11"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln w="15875">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -14549,36 +14947,14 @@
           </c:marker>
           <c:dPt>
             <c:idx val="0"/>
-            <c:marker>
-              <c:symbol val="diamond"/>
-              <c:size val="10"/>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="diamond"/>
-              <c:size val="10"/>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="diamond"/>
-              <c:size val="10"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-                <a:ln w="12700">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                </a:ln>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:xVal>
@@ -14627,11 +15003,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-800315552"/>
-        <c:axId val="-800180480"/>
+        <c:axId val="-2078272784"/>
+        <c:axId val="-2078268752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-800315552"/>
+        <c:axId val="-2078272784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -14660,7 +15036,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -14681,8 +15057,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.44208777245626"/>
-              <c:y val="0.884666489503056"/>
+              <c:x val="0.394554871623606"/>
+              <c:y val="0.921703150026695"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -14720,12 +15096,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-800180480"/>
+        <c:crossAx val="-2078268752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-800180480"/>
+        <c:axId val="-2078268752"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -14754,7 +15130,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1800" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -14775,8 +15151,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.01542328464517"/>
-              <c:y val="0.2944153517536"/>
+              <c:x val="0.00628235321214494"/>
+              <c:y val="0.294415331535711"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -14814,7 +15190,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-800315552"/>
+        <c:crossAx val="-2078272784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14828,42 +15204,6 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.706801518202194"/>
-          <c:y val="0.416795040899292"/>
-          <c:w val="0.199275607574434"/>
-          <c:h val="0.357467196897363"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr>
-              <a:latin typeface="Arial" charset="0"/>
-              <a:ea typeface="Arial" charset="0"/>
-              <a:cs typeface="Arial" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
@@ -15501,11 +15841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-323625728"/>
-        <c:axId val="-763249712"/>
+        <c:axId val="-2079231536"/>
+        <c:axId val="-2079227776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-323625728"/>
+        <c:axId val="-2079231536"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -15576,12 +15916,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-763249712"/>
+        <c:crossAx val="-2079227776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-763249712"/>
+        <c:axId val="-2079227776"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -15659,7 +15999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-323625728"/>
+        <c:crossAx val="-2079231536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17984,10 +18324,10 @@
       <xdr:rowOff>177820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596840</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>37980</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18009,15 +18349,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>20</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>184040</xdr:rowOff>
+      <xdr:colOff>533420</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>291880</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>56800</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18138,16 +18478,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>444640</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>177760</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>343040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12660</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>177400</xdr:rowOff>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18198,16 +18538,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>174900</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>187600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>5280</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>51780</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>165280</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18348,16 +18688,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>88920</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12880</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>584220</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76380</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>228220</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>38080</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>50420</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20277,7 +20617,7 @@
   <dimension ref="A1:AML58"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -44631,7 +44971,7 @@
         <v>25</v>
       </c>
       <c r="M54" s="27">
-        <f t="shared" ref="K54:O54" si="22">AVERAGE(Y1:Y51)</f>
+        <f t="shared" ref="M54:O54" si="22">AVERAGE(Y1:Y51)</f>
         <v>3.375922184313672</v>
       </c>
       <c r="N54" s="27">
@@ -47767,8 +48107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y234"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AC49" sqref="AC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51267,8 +51607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -51681,7 +52021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -52499,8 +52839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C48:AB61"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52655,7 +52995,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>